<commit_message>
script to evaluate training progress on all checkpoints in a folder
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656444CE-4B96-2A41-B4BF-7319431C0E37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC13E3-1E88-1845-843C-00BC832150B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="33540" windowHeight="20540" xr2:uid="{CD6B5847-7FE4-A944-B377-C39C60B45970}"/>
+    <workbookView xWindow="4860" yWindow="460" windowWidth="33540" windowHeight="21140" xr2:uid="{CD6B5847-7FE4-A944-B377-C39C60B45970}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
   <si>
     <t>6x100x25_best</t>
   </si>
   <si>
     <t>mcts=50, cpuct=1.0, temp=0</t>
-  </si>
-  <si>
-    <t>checkpoint_129</t>
   </si>
   <si>
     <t>"</t>
@@ -70,9 +68,6 @@
     <t>(Agent's perspective)</t>
   </si>
   <si>
-    <t>checkpoint_139</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -82,7 +77,7 @@
     <t>chainer</t>
   </si>
   <si>
-    <t>running on wdfl34316786a in screen pit0</t>
+    <t>mixed up draws and losses?</t>
   </si>
 </sst>
 </file>
@@ -119,7 +114,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +124,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -174,7 +181,20 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -186,13 +206,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,6 +221,992 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>260</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2B2-0C4E-9679-6CFFC2270140}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="909739535"/>
+        <c:axId val="909741215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="909739535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="909741215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="909741215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="909739535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>78154</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>263769</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>106485</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C115C9-E30F-2948-8810-9EFDA3883A94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E92D2C3-FF2B-C140-9BB5-E5A03D297275}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -527,50 +1526,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>15</v>
+      <c r="I1" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
+      <c r="A3" s="4">
+        <v>129</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -594,11 +1593,13 @@
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
+      <c r="A4" s="4">
+        <v>139</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -616,13 +1617,15 @@
         <v>24</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" ref="G4:G23" si="0">(D4-E4)/SUM(D4:F4)</f>
+        <f t="shared" ref="G4:G29" si="0">(D4-E4)/SUM(D4:F4)</f>
         <v>0.76</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4">
@@ -648,9 +1651,11 @@
         <v>0.54</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4">
@@ -676,7 +1681,7 @@
         <v>0.97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -704,7 +1709,7 @@
         <v>0.7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -732,7 +1737,7 @@
         <v>0.6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -760,7 +1765,7 @@
         <v>0.04</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -772,7 +1777,7 @@
         <v>149</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
         <v>62</v>
@@ -788,7 +1793,7 @@
         <v>0.24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -800,7 +1805,7 @@
         <v>155</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1">
         <v>50</v>
@@ -816,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -844,7 +1849,7 @@
         <v>0.7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -872,7 +1877,7 @@
         <v>0.86</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -886,13 +1891,13 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="14">
         <v>85</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="12">
         <v>15</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="12">
         <v>0</v>
       </c>
       <c r="G14" s="11">
@@ -900,7 +1905,7 @@
         <v>0.7</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -913,13 +1918,13 @@
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="14">
         <v>93</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="12">
         <v>7</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="12">
         <v>0</v>
       </c>
       <c r="G15" s="11">
@@ -927,7 +1932,7 @@
         <v>0.86</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -937,16 +1942,16 @@
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="12">
         <v>64</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="12">
         <v>36</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="12">
         <v>0</v>
       </c>
       <c r="G16" s="10">
@@ -963,16 +1968,16 @@
       <c r="B17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="C17" s="12">
+        <v>2</v>
+      </c>
+      <c r="D17" s="12">
         <v>50</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="12">
         <v>50</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="12">
         <v>0</v>
       </c>
       <c r="G17" s="10">
@@ -989,16 +1994,16 @@
       <c r="B18" s="6">
         <v>210</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="17">
+      <c r="C18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="12">
         <v>38</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="12">
         <v>62</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="12">
         <v>0</v>
       </c>
       <c r="G18" s="11">
@@ -1013,16 +2018,16 @@
       <c r="B19" s="6">
         <v>196</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="17">
+      <c r="C19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="12">
         <v>48</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="12">
         <v>52</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="12">
         <v>0</v>
       </c>
       <c r="G19" s="11">
@@ -1034,16 +2039,19 @@
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="17">
+      <c r="B20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="12">
         <v>16</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="12">
         <v>84</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="12">
         <v>0</v>
       </c>
       <c r="G20" s="11">
@@ -1053,29 +2061,26 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="17">
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="12">
         <v>85</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="12">
         <v>15</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="12">
         <v>0</v>
       </c>
       <c r="G21" s="11">
         <f t="shared" si="0"/>
         <v>0.7</v>
-      </c>
-      <c r="I21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1088,13 +2093,13 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="12">
         <v>43</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="12">
         <v>57</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="12">
         <v>0</v>
       </c>
       <c r="G22" s="11">
@@ -1112,13 +2117,13 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="12">
         <v>38</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="12">
         <v>62</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="12">
         <v>0</v>
       </c>
       <c r="G23" s="11">
@@ -1131,10 +2136,23 @@
         <v>230</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>1</v>
+      </c>
+      <c r="D24" s="12">
+        <v>18</v>
+      </c>
+      <c r="E24" s="12">
+        <v>82</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.64</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1142,10 +2160,119 @@
         <v>230</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="12">
+        <v>21</v>
+      </c>
+      <c r="E25" s="12">
+        <v>79</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="6">
+        <v>260</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
+        <v>29</v>
+      </c>
+      <c r="E26" s="12">
+        <v>71</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="6">
+        <v>260</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="12">
         <v>17</v>
       </c>
-      <c r="C25">
-        <v>2</v>
+      <c r="E27" s="12">
+        <v>83</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="6">
+        <v>260</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="15">
+        <v>68</v>
+      </c>
+      <c r="E28" s="12">
+        <v>32</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="6">
+        <v>260</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="15">
+        <v>56</v>
+      </c>
+      <c r="E29" s="12">
+        <v>44</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -1163,4 +2290,431 @@
     <ignoredError sqref="G13 G3:G11" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265D7CDA-F7A3-0243-A8C6-9D5FFF6C0374}">
+  <dimension ref="A2:G18"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" activeCellId="1" sqref="A2:A18 G2:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4">
+        <v>129</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>73</v>
+      </c>
+      <c r="G2" s="9">
+        <f>(D2-E2)/SUM(D2:F2)</f>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4">
+        <v>139</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>76</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>24</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G18" si="0">(D3-E3)/SUM(D3:F3)</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4">
+        <v>146</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>46</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4">
+        <v>149</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>97</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4">
+        <v>149</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>85</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4">
+        <v>155</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>40</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4">
+        <v>155</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>52</v>
+      </c>
+      <c r="E8" s="1">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4">
+        <v>196</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <f>(D9-E9)/SUM(D9:F9)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4">
+        <v>196</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>93</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4">
+        <v>196</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>85</v>
+      </c>
+      <c r="E11" s="12">
+        <v>15</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <f>(D11-E11)/SUM(D11:F11)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4">
+        <v>196</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>93</v>
+      </c>
+      <c r="E12" s="12">
+        <v>7</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <f>(D12-E12)/SUM(D12:F12)</f>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5">
+        <v>210</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>64</v>
+      </c>
+      <c r="E13" s="12">
+        <v>36</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5">
+        <v>210</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12">
+        <v>50</v>
+      </c>
+      <c r="E14" s="12">
+        <v>50</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4">
+        <v>230</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>43</v>
+      </c>
+      <c r="E15" s="12">
+        <v>57</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4">
+        <v>230</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="12">
+        <v>38</v>
+      </c>
+      <c r="E16" s="12">
+        <v>62</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6">
+        <v>260</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>68</v>
+      </c>
+      <c r="E17" s="12">
+        <v>32</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6">
+        <v>260</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15">
+        <v>56</v>
+      </c>
+      <c r="E18" s="12">
+        <v>44</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
eval.py: reset MCTS after each game
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC13E3-1E88-1845-843C-00BC832150B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B7937E-CF11-5644-9C0E-278C538E6542}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="460" windowWidth="33540" windowHeight="21140" xr2:uid="{CD6B5847-7FE4-A944-B377-C39C60B45970}"/>
+    <workbookView xWindow="63440" yWindow="4700" windowWidth="35660" windowHeight="21180" activeTab="2" xr2:uid="{CD6B5847-7FE4-A944-B377-C39C60B45970}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
   <si>
     <t>6x100x25_best</t>
   </si>
@@ -78,6 +79,61 @@
   </si>
   <si>
     <t>mixed up draws and losses?</t>
+  </si>
+  <si>
+    <t>player1</t>
+  </si>
+  <si>
+    <t>player2</t>
+  </si>
+  <si>
+    <t>wins</t>
+  </si>
+  <si>
+    <t>losses</t>
+  </si>
+  <si>
+    <t>draws</t>
+  </si>
+  <si>
+    <t>game_results</t>
+  </si>
+  <si>
+    <t>pytorch</t>
+  </si>
+  <si>
+    <t>[-1, -1, -1, -1, -1, 1, -1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[-1, -1, -1, -1, -1, 1, -1, 1, 1, 1, 1, -1, -1, -1, -1, 1, 1, 1, 1, 1, -1, -1, -1, 1, 1, 1, 1, 1, 1, -1]</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>pit</t>
+  </si>
+  <si>
+    <t>battle</t>
+  </si>
+  <si>
+    <t>ckpt 340</t>
+  </si>
+  <si>
+    <t>train_progress</t>
+  </si>
+  <si>
+    <t>[-1  1 -1  1  1 -1  1  1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1  1 -1
+ -1  1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1
+ -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1  1  1
+  1  1  1  1  1  1  1  1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1 -1
+ -1 -1 -1 -1]</t>
+  </si>
+  <si>
+    <t>perspective: p1</t>
+  </si>
+  <si>
+    <t>[-1, 1, -1, 1, 1, -1, 1, 1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, 1, -1, -1, 1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1, -1]</t>
   </si>
 </sst>
 </file>
@@ -114,7 +170,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +195,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,11 +210,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -191,6 +262,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -205,6 +279,12 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -300,59 +380,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$18</c:f>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>129</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>146</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>196</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>260</c:v>
                 </c:pt>
               </c:numCache>
@@ -360,60 +410,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$G$2:$G$18</c:f>
+              <c:f>Sheet2!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.54</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
-                  <c:v>0.97</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.04</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.86</c:v>
+                  <c:v>-0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.28000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.24</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>0.36</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,7 +1200,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>263769</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>106485</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1508,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E92D2C3-FF2B-C140-9BB5-E5A03D297275}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1526,13 +1546,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -1544,28 +1564,28 @@
       <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="17" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4">
@@ -1667,7 +1687,7 @@
       <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="16">
         <v>97</v>
       </c>
       <c r="E6" s="1">
@@ -1695,7 +1715,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="16">
         <v>85</v>
       </c>
       <c r="E7" s="1">
@@ -2294,10 +2314,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265D7CDA-F7A3-0243-A8C6-9D5FFF6C0374}">
-  <dimension ref="A2:G18"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" activeCellId="1" sqref="A2:A18 G2:G18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2306,76 +2326,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="4">
-        <v>129</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>73</v>
-      </c>
-      <c r="G2" s="9">
-        <f>(D2-E2)/SUM(D2:F2)</f>
-        <v>0.27</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4">
-        <v>139</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>76</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>24</v>
-      </c>
-      <c r="G3" s="9">
-        <f t="shared" ref="G3:G18" si="0">(D3-E3)/SUM(D3:F3)</f>
-        <v>0.76</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4">
-        <v>146</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>54</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>46</v>
-      </c>
-      <c r="G4" s="9">
-        <f t="shared" si="0"/>
-        <v>0.54</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
@@ -2385,25 +2360,25 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>0.97</v>
+        <f t="shared" ref="G5:G11" si="0">(D5-E5)/SUM(D5:F5)</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -2412,46 +2387,46 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
+        <f>(D7-E7)/SUM(D7:F7)</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -2459,262 +2434,285 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
-        <v>52</v>
-      </c>
-      <c r="E8" s="1">
-        <v>48</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="D8" s="14">
+        <v>85</v>
+      </c>
+      <c r="E8" s="12">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <f>(D8-E8)/SUM(D8:F8)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5">
+        <v>210</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>64</v>
+      </c>
+      <c r="E9" s="12">
+        <v>36</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4">
-        <v>196</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>85</v>
-      </c>
-      <c r="E9" s="1">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <f>(D9-E9)/SUM(D9:F9)</f>
-        <v>0.7</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>93</v>
-      </c>
-      <c r="E10" s="1">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="4">
-        <v>196</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="D11" s="14">
-        <v>85</v>
-      </c>
-      <c r="E11" s="12">
-        <v>15</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11">
-        <f>(D11-E11)/SUM(D11:F11)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="4">
-        <v>196</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14">
-        <v>93</v>
-      </c>
-      <c r="E12" s="12">
-        <v>7</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
-        <f>(D12-E12)/SUM(D12:F12)</f>
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5">
-        <v>210</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
-        <v>1</v>
-      </c>
-      <c r="D13" s="12">
-        <v>64</v>
-      </c>
-      <c r="E13" s="12">
-        <v>36</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10">
-        <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5">
-        <v>210</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
-        <v>2</v>
-      </c>
-      <c r="D14" s="12">
-        <v>50</v>
-      </c>
-      <c r="E14" s="12">
-        <v>50</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="4">
-        <v>230</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="12">
+      <c r="D10" s="12">
         <v>43</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E10" s="12">
         <v>57</v>
       </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="4">
-        <v>230</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="12">
-        <v>38</v>
-      </c>
-      <c r="E16" s="12">
-        <v>62</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" si="0"/>
-        <v>-0.24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="6">
+    <row r="11" spans="1:7">
+      <c r="A11" s="6">
         <v>260</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D11" s="15">
         <v>68</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E11" s="12">
         <v>32</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
         <v>0.36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="6">
-        <v>260</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="15">
-        <v>56</v>
-      </c>
-      <c r="E18" s="12">
-        <v>44</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D06E71-337F-804D-BA95-43521D5D9355}">
+  <dimension ref="A4:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
+    <col min="5" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7">
+      <c r="D4" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>83</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="85">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>83</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>83</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>